<commit_message>
Detect Events fn created, updated index files
- Detect events function scans distP and distQ
- updated index files to include thresholds
</commit_message>
<xml_diff>
--- a/ML/Windows_H4.xlsx
+++ b/ML/Windows_H4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7820"/>
   </bookViews>
   <sheets>
     <sheet name="H4-1" sheetId="1" r:id="rId1"/>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:R1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1081,7 +1081,7 @@
         <v>3.7589999999999999</v>
       </c>
       <c r="R5" s="3">
-        <v>4.4950000000000001</v>
+        <v>4.7460000000000004</v>
       </c>
       <c r="S5" s="29"/>
       <c r="T5" s="21"/>
@@ -2719,7 +2719,7 @@
         <v>1</v>
       </c>
       <c r="Q34" s="3">
-        <v>4.944</v>
+        <v>5.4690000000000003</v>
       </c>
       <c r="R34" s="3">
         <v>1.8979999999999999</v>
@@ -3001,10 +3001,10 @@
         <v>1</v>
       </c>
       <c r="Q39" s="3">
-        <v>4.59</v>
+        <v>4.6289999999999996</v>
       </c>
       <c r="R39" s="3">
-        <v>4.6669999999999998</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.35">
@@ -3297,7 +3297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q80" sqref="Q80"/>
     </sheetView>
   </sheetViews>

</xml_diff>